<commit_message>
Updated results for NN with latest feature vector with dimensionality reduction
Updated results for NN with latest feature vector with dimensionality
reduction
</commit_message>
<xml_diff>
--- a/results/Neural_Network_Results.xlsx
+++ b/results/Neural_Network_Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Algorithm</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Activation</t>
   </si>
   <si>
-    <t>Hidden Layers</t>
-  </si>
-  <si>
     <t>stochastic gradient Descent</t>
   </si>
   <si>
@@ -37,7 +34,13 @@
     <t>Error Test</t>
   </si>
   <si>
-    <t>Nodes</t>
+    <t>(5,3)</t>
+  </si>
+  <si>
+    <t>HL Nodes</t>
+  </si>
+  <si>
+    <t>Logistic</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,12 +419,11 @@
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,98 +431,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="D2">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.34100000000000003</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="F2">
-        <v>0.46899999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="E3">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="F3">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="F4">
-        <v>0.378</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>0.248</v>
-      </c>
-      <c r="F5">
-        <v>0.39800000000000002</v>
+        <v>0.44700000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>